<commit_message>
identified another type of snes extension
</commit_message>
<xml_diff>
--- a/hardware/munia.xlsx
+++ b/hardware/munia.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frank\Desktop\workspace\munia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frank\Desktop\workspace\munia\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4FBC22BF-FF61-48F0-AE40-3BE2F39A5B9E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="27795" windowHeight="14640" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="27795" windowHeight="14640" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="components" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="160">
   <si>
     <t>Component</t>
   </si>
@@ -501,12 +502,15 @@
   </si>
   <si>
     <t>w/ white wire</t>
+  </si>
+  <si>
+    <t>SNES cable 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$€-413]\ #,##0.00"/>
@@ -846,16 +850,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>236481</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>59119</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>170793</xdr:rowOff>
+      <xdr:rowOff>151086</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>350914</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>258949</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>34674</xdr:rowOff>
+      <xdr:rowOff>14967</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -885,7 +889,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5590188" y="9327931"/>
+          <a:off x="5577050" y="9308224"/>
           <a:ext cx="2242778" cy="625881"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -914,7 +918,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>454572</xdr:colOff>
+      <xdr:colOff>546538</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>174735</xdr:rowOff>
     </xdr:to>
@@ -968,16 +972,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>321880</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>124811</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>26276</xdr:rowOff>
+      <xdr:rowOff>6569</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>390509</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>278837</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>69961</xdr:rowOff>
+      <xdr:rowOff>50254</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1007,7 +1011,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5675587" y="9945414"/>
+          <a:off x="5642742" y="9925707"/>
           <a:ext cx="2196974" cy="615185"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1350,7 +1354,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1499,12 +1503,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E7" r:id="rId1"/>
-    <hyperlink ref="E6" r:id="rId2"/>
-    <hyperlink ref="E5" r:id="rId3"/>
-    <hyperlink ref="E4" r:id="rId4"/>
-    <hyperlink ref="E2" r:id="rId5"/>
-    <hyperlink ref="E3" r:id="rId6"/>
+    <hyperlink ref="E7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E6" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E3" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId7"/>
@@ -1512,7 +1516,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1944,7 +1948,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H92"/>
   <sheetViews>
     <sheetView topLeftCell="A24" workbookViewId="0">
@@ -3161,7 +3165,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3417,7 +3421,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3429,11 +3433,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3443,16 +3447,17 @@
     <col min="3" max="3" width="11.42578125" customWidth="1"/>
     <col min="4" max="5" width="14.85546875" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="14" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>137</v>
       </c>
@@ -3477,8 +3482,11 @@
       <c r="H3" s="30" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="30" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="31">
         <v>1</v>
       </c>
@@ -3497,8 +3505,11 @@
       <c r="H4" s="35" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="31">
         <v>2</v>
       </c>
@@ -3517,8 +3528,11 @@
       <c r="H5" s="37" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="37" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="31">
         <v>3</v>
       </c>
@@ -3537,8 +3551,11 @@
       <c r="H6" s="33" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="33" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="31">
         <v>4</v>
       </c>
@@ -3557,8 +3574,11 @@
       <c r="H7" s="27" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="31">
         <v>5</v>
       </c>
@@ -3579,8 +3599,9 @@
       </c>
       <c r="G8" s="33"/>
       <c r="H8" s="33"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="33"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="31">
         <v>6</v>
       </c>
@@ -3597,8 +3618,9 @@
       <c r="F9" s="33"/>
       <c r="G9" s="33"/>
       <c r="H9" s="33"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="33"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="31">
         <v>7</v>
       </c>
@@ -3619,8 +3641,9 @@
       </c>
       <c r="G10" s="33"/>
       <c r="H10" s="33"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="33"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="31">
         <v>8</v>
       </c>
@@ -3645,8 +3668,11 @@
       <c r="H11" s="39" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="43" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D12" s="1" t="s">
         <v>151</v>
       </c>
@@ -3660,12 +3686,12 @@
         <v>158</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:9" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="14" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="46" t="s">
         <v>134</v>
       </c>
@@ -3680,7 +3706,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="49"/>
       <c r="B15" s="49"/>
       <c r="C15" s="8"/>
@@ -3689,7 +3715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="45"/>
       <c r="B16" s="45"/>
       <c r="C16" s="9"/>
@@ -3868,7 +3894,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
         <v>137</v>
       </c>
@@ -3880,7 +3906,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="18">
         <v>1</v>
       </c>
@@ -3894,7 +3920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="18">
         <v>2</v>
       </c>
@@ -3908,7 +3934,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="18">
         <v>3</v>
       </c>
@@ -3922,17 +3948,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:7" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="14" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="23" t="s">
         <v>137</v>
       </c>
@@ -3948,11 +3974,14 @@
       <c r="E43" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="F43" s="20" t="s">
+      <c r="F43" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="G43" s="20" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="18">
         <v>1</v>
       </c>
@@ -3968,11 +3997,14 @@
       <c r="E44" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="F44" s="18">
+      <c r="F44" s="43" t="s">
+        <v>111</v>
+      </c>
+      <c r="G44" s="18">
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="18">
         <v>2</v>
       </c>
@@ -3988,11 +4020,14 @@
       <c r="E45" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="F45" s="18">
+      <c r="F45" s="37" t="s">
+        <v>123</v>
+      </c>
+      <c r="G45" s="18">
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="18">
         <v>3</v>
       </c>
@@ -4008,11 +4043,14 @@
       <c r="E46" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="F46" s="18">
+      <c r="F46" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="G46" s="18">
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="18">
         <v>4</v>
       </c>
@@ -4028,11 +4066,14 @@
       <c r="E47" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="F47" s="18">
+      <c r="F47" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="G47" s="18">
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="18">
         <v>5</v>
       </c>
@@ -4048,7 +4089,10 @@
       <c r="E48" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="F48" s="18">
+      <c r="F48" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="G48" s="18">
         <v>1</v>
       </c>
     </row>

</xml_diff>